<commit_message>
Se agrego Vista de Restorant
</commit_message>
<xml_diff>
--- a/pantallas/medidas.xlsx
+++ b/pantallas/medidas.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2700" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="restaurant" sheetId="2" r:id="rId2"/>
+    <sheet name="retaurant_proudct" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,12 +26,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>alto pantalla</t>
   </si>
   <si>
     <t xml:space="preserve">bloque1 </t>
+  </si>
+  <si>
+    <t>alto</t>
+  </si>
+  <si>
+    <t>acho</t>
+  </si>
+  <si>
+    <t>bottom card</t>
+  </si>
+  <si>
+    <t>imagen sup</t>
+  </si>
+  <si>
+    <t>radio</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>alt card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alt add </t>
+  </si>
+  <si>
+    <t>slider w</t>
+  </si>
+  <si>
+    <t>anc</t>
   </si>
 </sst>
 </file>
@@ -65,8 +97,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -374,7 +407,7 @@
         <v>26</v>
       </c>
       <c r="C3">
-        <f>B3/B$1*100</f>
+        <f t="shared" ref="C3:C15" si="0">B3/B$1*100</f>
         <v>4.6017699115044248</v>
       </c>
       <c r="E3">
@@ -393,7 +426,7 @@
         <v>15.75</v>
       </c>
       <c r="C4">
-        <f>B4/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>2.7876106194690267</v>
       </c>
     </row>
@@ -402,7 +435,7 @@
         <v>24.59</v>
       </c>
       <c r="C5">
-        <f>B5/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>4.3522123893805311</v>
       </c>
     </row>
@@ -411,7 +444,7 @@
         <v>21.16</v>
       </c>
       <c r="C6">
-        <f>B6/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>3.7451327433628321</v>
       </c>
     </row>
@@ -420,7 +453,7 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <f>B7/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>2.6548672566371683</v>
       </c>
     </row>
@@ -429,7 +462,7 @@
         <v>14.27</v>
       </c>
       <c r="C8">
-        <f>B8/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>2.5256637168141594</v>
       </c>
     </row>
@@ -438,7 +471,7 @@
         <v>22.64</v>
       </c>
       <c r="C9">
-        <f>B9/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>4.0070796460176989</v>
       </c>
     </row>
@@ -447,7 +480,7 @@
         <v>37.9</v>
       </c>
       <c r="C10">
-        <f>B10/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>6.7079646017699108</v>
       </c>
     </row>
@@ -456,7 +489,7 @@
         <v>33.5</v>
       </c>
       <c r="C11">
-        <f>B11/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>5.9292035398230087</v>
       </c>
     </row>
@@ -465,7 +498,7 @@
         <v>18.7</v>
       </c>
       <c r="C12">
-        <f>B12/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>3.3097345132743357</v>
       </c>
     </row>
@@ -474,7 +507,7 @@
         <v>19</v>
       </c>
       <c r="C13">
-        <f>B13/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>3.3628318584070795</v>
       </c>
     </row>
@@ -483,7 +516,7 @@
         <v>26.58</v>
       </c>
       <c r="C14">
-        <f>B14/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>4.7044247787610614</v>
       </c>
     </row>
@@ -492,7 +525,7 @@
         <v>15.18</v>
       </c>
       <c r="C15">
-        <f>B15/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>2.686725663716814</v>
       </c>
     </row>
@@ -500,4 +533,191 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>149</v>
+      </c>
+      <c r="C4" s="1">
+        <f>B4/B$1*100</f>
+        <v>34.018264840182653</v>
+      </c>
+      <c r="D4">
+        <f>B1-B4</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>295</v>
+      </c>
+      <c r="C5" s="1">
+        <f>B5/B$1*100</f>
+        <v>67.351598173515981</v>
+      </c>
+      <c r="D5">
+        <f>B1*C5/100</f>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <f>B6/B$1*100</f>
+        <v>2.2831050228310499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>72.88</v>
+      </c>
+      <c r="C7" s="1">
+        <f>B7/B$1*100</f>
+        <v>16.639269406392692</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1">
+        <f>B8/B$1*100</f>
+        <v>6.6210045662100452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1">
+        <f>B9/B$1*100</f>
+        <v>14.15525114155251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1">
+        <v>560</v>
+      </c>
+      <c r="E1">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>264</v>
+      </c>
+      <c r="E2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>314</v>
+      </c>
+      <c r="C3">
+        <f>B3*100/B$1</f>
+        <v>56.071428571428569</v>
+      </c>
+      <c r="E3">
+        <v>42</v>
+      </c>
+      <c r="F3">
+        <f>E3/E2*100</f>
+        <v>16.216216216216218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <f>B4*100/B$1</f>
+        <v>6.7857142857142856</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>144</v>
+      </c>
+      <c r="C5">
+        <f>B5*100/B2</f>
+        <v>54.545454545454547</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego My Order View
</commit_message>
<xml_diff>
--- a/pantallas/medidas.xlsx
+++ b/pantallas/medidas.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2700" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2700" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="restaurant" sheetId="2" r:id="rId2"/>
     <sheet name="retaurant_proudct" sheetId="3" r:id="rId3"/>
+    <sheet name="my_order" sheetId="4" r:id="rId4"/>
+    <sheet name="near_me" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>alto pantalla</t>
   </si>
@@ -62,13 +64,25 @@
   </si>
   <si>
     <t>anc</t>
+  </si>
+  <si>
+    <t>ancho</t>
+  </si>
+  <si>
+    <t>dispositivo</t>
+  </si>
+  <si>
+    <t>buttons</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,13 +90,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -97,9 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,7 +603,7 @@
         <v>149</v>
       </c>
       <c r="C4" s="1">
-        <f>B4/B$1*100</f>
+        <f t="shared" ref="C4:C9" si="0">B4/B$1*100</f>
         <v>34.018264840182653</v>
       </c>
       <c r="D4">
@@ -589,7 +619,7 @@
         <v>295</v>
       </c>
       <c r="C5" s="1">
-        <f>B5/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>67.351598173515981</v>
       </c>
       <c r="D5">
@@ -605,7 +635,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <f>B6/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>2.2831050228310499</v>
       </c>
     </row>
@@ -614,7 +644,7 @@
         <v>72.88</v>
       </c>
       <c r="C7" s="1">
-        <f>B7/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>16.639269406392692</v>
       </c>
     </row>
@@ -623,7 +653,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="1">
-        <f>B8/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>6.6210045662100452</v>
       </c>
     </row>
@@ -632,7 +662,7 @@
         <v>62</v>
       </c>
       <c r="C9" s="1">
-        <f>B9/B$1*100</f>
+        <f t="shared" si="0"/>
         <v>14.15525114155251</v>
       </c>
     </row>
@@ -646,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -720,4 +750,117 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>385</v>
+      </c>
+      <c r="C2" s="2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3">
+        <f>B3/B2*100</f>
+        <v>4.9350649350649354</v>
+      </c>
+      <c r="C4" s="3">
+        <f>C3/C2*100</f>
+        <v>39.325842696629216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>460</v>
+      </c>
+      <c r="C2" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3">
+        <f>B3/B2*100</f>
+        <v>3.6956521739130435</v>
+      </c>
+      <c r="C4" s="3">
+        <f>C3/C2*100</f>
+        <v>60.377358490566039</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>